<commit_message>
Updated Schedule, April 30th
</commit_message>
<xml_diff>
--- a/Group 4 General Schedule Ver4.26.xlsx
+++ b/Group 4 General Schedule Ver4.26.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dldms\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Group4Project\project-group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE6C878-6225-4A6B-B72D-F84A28F5EEB7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE5CE3E-D56D-4A44-A8AB-31654F41EE9C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="7428" xr2:uid="{97468DF9-BE6D-47DA-8544-6EE465DD669F}"/>
   </bookViews>
@@ -113,11 +113,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Write an article on the page. 
-Responsive part of the page
-has to be done. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Finish basic background, 
 basic features. 
 </t>
@@ -125,12 +120,6 @@
   <si>
     <t xml:space="preserve">Design the tower visuals, 
 design background of the game
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Host the webpage and 
-find the right link for the
- page. 
 </t>
   </si>
   <si>
@@ -174,15 +163,42 @@
 Review Javascript from COMP1527</t>
   </si>
   <si>
-    <t xml:space="preserve">Assist the art expert (William)
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Choose Game Engine.
  </t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>QA test on the first version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assist the art expert
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design animations, 
+</t>
+  </si>
+  <si>
+    <t>Game development</t>
+  </si>
+  <si>
+    <t>Finish first version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final touch on the art. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish first version, 
+QA test the game. </t>
+  </si>
+  <si>
+    <t>Media, 
+QA tester
+Advertisement, 
+Presentation,
+Artist 2</t>
   </si>
   <si>
     <r>
@@ -194,8 +210,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">This schedule can be changed any time according to the actual workload done.
-Claim for overly imposed workload can be written on slack and schedule can change. </t>
+      <t>This schedule can be changed any time according to the actual workload done.
+Claim for overly imposed workload can be written on slack and schedule can change. 
+QA log link: https://docs.google.com/document/d/1xh_44jDLhRtUZO6BpEWbmFri1WRelBw3NhSJnzZkNZA/edit?usp=sharing</t>
     </r>
     <r>
       <rPr>
@@ -210,39 +227,27 @@
     </r>
   </si>
   <si>
-    <t>QA test on the first version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assist the art expert
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design animations, 
-</t>
-  </si>
-  <si>
-    <t>Finish the page. 
+    <t>Make the page responsive. 
+Make 3 pages : 
+Home (contain the game) 
+Food Waste reduction (Cover the details on the messages that we are trying to deliver through the game) , 
+Game Manual (Detailed explanation on game story, tower features, food characteristics, and so on)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assist the art part (with William)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Host the webpage and 
+find the right link for the
+ page. 
+Implement MySQL and some hosting features mentioned in the lecture. 
+</t>
+  </si>
+  <si>
+    <t>Fill the detailed contents on the page. 
+Finish the page. 
 Game development</t>
-  </si>
-  <si>
-    <t>Game development</t>
-  </si>
-  <si>
-    <t>Finish first version</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final touch on the art. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finish first version, 
-QA test the game. </t>
-  </si>
-  <si>
-    <t>Media, 
-QA tester
-Advertisement, 
-Presentation,
-Artist 2</t>
   </si>
 </sst>
 </file>
@@ -326,9 +331,6 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -345,6 +347,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -708,7 +713,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,239 +728,239 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Web page and updated schedule for the group
</commit_message>
<xml_diff>
--- a/Group 4 General Schedule Ver4.26.xlsx
+++ b/Group 4 General Schedule Ver4.26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Group4Project\project-group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE5CE3E-D56D-4A44-A8AB-31654F41EE9C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D062FA17-DA4D-4449-8896-3AB4B6D80D68}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15312" windowHeight="7428" xr2:uid="{97468DF9-BE6D-47DA-8544-6EE465DD669F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>General Schedule</t>
   </si>
@@ -110,16 +110,6 @@
     <t xml:space="preserve">Design the protagonist, 
 Design the logo, 
 Design the game title, 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finish basic background, 
-basic features. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design the tower visuals, 
-design background of the game
 </t>
   </si>
   <si>
@@ -174,10 +164,6 @@
   </si>
   <si>
     <t xml:space="preserve">Assist the art expert
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design animations, 
 </t>
   </si>
   <si>
@@ -227,27 +213,50 @@
     </r>
   </si>
   <si>
-    <t>Make the page responsive. 
-Make 3 pages : 
-Home (contain the game) 
-Food Waste reduction (Cover the details on the messages that we are trying to deliver through the game) , 
-Game Manual (Detailed explanation on game story, tower features, food characteristics, and so on)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Assist the art part (with William)
 </t>
+  </si>
+  <si>
+    <t>Fill the detailed contents on the page. 
+Finish the page. 
+Game development</t>
   </si>
   <si>
     <t xml:space="preserve">Host the webpage and 
 find the right link for the
  page. 
-Implement MySQL and some hosting features mentioned in the lecture. 
+Implement MySQL and some hosting features mentioned in the lecture.
+Add money feature in the game.  
 </t>
   </si>
   <si>
-    <t>Fill the detailed contents on the page. 
-Finish the page. 
-Game development</t>
+    <t xml:space="preserve">Finish game prototype, 
+UI design, 
+Game lobby screen, 
+Change UI sccording to the size of the visual that William created. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design the tower visuals, 
+design background of the game
+Finish PNG image of the game background, 
+Finish png image of at least half of the towers. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish visuals for all the towers. 
+Design animations,  of towers composting food. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read the code of 
+the actual game 
+and keep up 
+with what's going
+ on. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write the contents on the page. Make Login page, 
+host it and link login to the database SQL. </t>
   </si>
 </sst>
 </file>
@@ -285,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -324,11 +333,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -351,11 +375,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="16">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -376,6 +406,178 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -398,16 +600,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{967DD519-3DDE-419F-9252-73F366C2533B}" name="Table1" displayName="Table1" ref="A2:G14" totalsRowCount="1" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{967DD519-3DDE-419F-9252-73F366C2533B}" name="Table1" displayName="Table1" ref="A2:G14" totalsRowCount="1" headerRowDxfId="7" tableBorderDxfId="15">
   <autoFilter ref="A2:G13" xr:uid="{31DF8158-4CC6-41C3-8A92-0B7E49CED26F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{2D9C6C32-EEB5-4D37-8BAC-767A996886DE}" name="Row" totalsRowLabel=" " totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{0A25985F-CE4A-4137-B903-A5C393D53C10}" name="David" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{D6FA6F6B-8D79-4159-969E-A5F626163230}" name="Tommy" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{72FEF8A4-56E9-49AD-B1BD-CD07237D4DBF}" name="Khide" totalsRowDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{FF5E7E45-64F7-4101-948D-86859E464EC8}" name="William" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7BA404D4-5DF0-4F76-9A41-4F48D8F06ECF}" name="Sagar" totalsRowDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{229A0120-B2F1-4633-9ACB-829FD4102AE2}" name="Everyone. " totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2D9C6C32-EEB5-4D37-8BAC-767A996886DE}" name="Row" totalsRowLabel=" " dataDxfId="14" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{0A25985F-CE4A-4137-B903-A5C393D53C10}" name="David" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{D6FA6F6B-8D79-4159-969E-A5F626163230}" name="Tommy" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{72FEF8A4-56E9-49AD-B1BD-CD07237D4DBF}" name="Khide" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FF5E7E45-64F7-4101-948D-86859E464EC8}" name="William" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7BA404D4-5DF0-4F76-9A41-4F48D8F06ECF}" name="Sagar" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{229A0120-B2F1-4633-9ACB-829FD4102AE2}" name="Everyone. " dataDxfId="8" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -713,7 +915,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,210 +941,212 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
+      <c r="E8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="G8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
@@ -953,7 +1157,7 @@
     </row>
     <row r="15" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>

</xml_diff>